<commit_message>
- Switched the "logkey" position from the beginning of the log message to the end - Removed unnecessary variables from "wait for..." activities - Added new comment for Digitize/Classify/Extract: "A/An <activity> that uses a paid license might incur extra costs when re-executing. This should be taken into consideration for the number of retries." - small reinforcement to the IKC Learning file - added a placeholder.txt in the exports folder - Config.xlsx had some updates with default endpoints for classification/extraction/digitization added - Config.xlsx had some updates regarding the required Shared folders (modern folders) in Orchestrator and the ActionCatalogs
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\UiPath\GitStudioTemplates\StudioTemplates\REFramework_DocumentUnderstanding\VB\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\GitProjects\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93947058-CBAF-4A40-86AA-09F1B0ACF82A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E1A97A-B6B6-4A2F-9AEF-A925D4C14E74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Project initialization started</t>
   </si>
   <si>
-    <t>Maximum number of execution attempts for a process step. Minimum value is 1</t>
-  </si>
-  <si>
     <t>LogMessage_DigitizationStarted</t>
   </si>
   <si>
@@ -165,15 +162,6 @@
     <t>StorageBucketFolderPath</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>UiPath public end-point for receipts</t>
-  </si>
-  <si>
-    <t>UiPath public end-point for invoices</t>
-  </si>
-  <si>
     <t>SplitFolder</t>
   </si>
   <si>
@@ -340,13 +328,64 @@
   </si>
   <si>
     <t>DocumentUnderstandingQueuePath</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsDigitize</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsClassify</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsExtract</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for the Extract step. Minimum value is 1. An Extractor that uses a paid license might incur extra costs when re-executing. This should be taken into consideration for the number of retries.</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for the Classify step. Minimum value is 1. A Classifier that uses a paid license might incur extra costs when re-executing. This should be taken into consideration when for the number of retries.</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for a process step. Minimum value is 1.</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for the Digitize step. Minimum value is 1.  An OCR engine that uses a paid license might incur extra costs when re-executing. This should be taken into consideration when for the number of retries.</t>
+  </si>
+  <si>
+    <t>TestAction</t>
+  </si>
+  <si>
+    <t>https://du.uipath.com/svc/intelligentkeywords</t>
+  </si>
+  <si>
+    <t>ClassifiactionEndpoint</t>
+  </si>
+  <si>
+    <t>IntelligentFormExtractorEndpoint</t>
+  </si>
+  <si>
+    <t>https://du.uipath.com/svc/intelligentforms</t>
+  </si>
+  <si>
+    <t>UiPath public endpoint for classification</t>
+  </si>
+  <si>
+    <t>UiPath public endpoint for Intelligent Form Extractor</t>
+  </si>
+  <si>
+    <t>UiPath public endpoint for receipts</t>
+  </si>
+  <si>
+    <t>UiPath public endpoint for invoices</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +410,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -718,7 +761,7 @@
   <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -799,18 +842,18 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -818,7 +861,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -826,75 +869,81 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -902,10 +951,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -913,26 +962,46 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1929,9 +1998,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1986,259 +2055,289 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
+        <v>104</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+        <v>60</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-    </row>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>98</v>
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>101</v>
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
+        <v>95</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
+        <v>96</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>102</v>
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>90</v>
+      <c r="A27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-    </row>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2247,960 +2346,967 @@
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3211,7 +3317,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3230,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3261,13 +3367,16 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added queue support for the DU Process
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A960908E-4741-4B77-90F3-BB608A30209D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11EB5D3-ED2F-4786-893E-BF650090481A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4548" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t>TestBucket</t>
   </si>
   <si>
-    <t>StorageBucketFolderPath</t>
-  </si>
-  <si>
     <t>SplitFolder</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>WarnMessage_DocumentProcessingFailure</t>
   </si>
   <si>
-    <t>Failed to process document. Exception:</t>
-  </si>
-  <si>
     <t>https://du.uipath.com/ie/invoices</t>
   </si>
   <si>
@@ -315,9 +309,6 @@
     <t>LogMessage_ClassificationFinished</t>
   </si>
   <si>
-    <t>Classification Finished.</t>
-  </si>
-  <si>
     <t>Data Extraction finished.</t>
   </si>
   <si>
@@ -373,6 +364,63 @@
   </si>
   <si>
     <t>UiPath public endpoint for invoices</t>
+  </si>
+  <si>
+    <t>StorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>Path to the directory, within the storage bucket, where validation actions should store data.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionItem</t>
+  </si>
+  <si>
+    <t>Get Transaction Item started</t>
+  </si>
+  <si>
+    <t>Classification Finished</t>
+  </si>
+  <si>
+    <t>LogMessage_SetTransactionProgress</t>
+  </si>
+  <si>
+    <t>LogMessage_SetTransactionStatusSuccess</t>
+  </si>
+  <si>
+    <t>LogMessage_SetTransactionStatusBRE</t>
+  </si>
+  <si>
+    <t>LogMessage_SetTransactionStatusSystemException</t>
+  </si>
+  <si>
+    <t>Transaction successful</t>
+  </si>
+  <si>
+    <t>Transaction failed due to Business Rule Exception:</t>
+  </si>
+  <si>
+    <t>Transaction failed due to System Exception:</t>
+  </si>
+  <si>
+    <t>Updating transaction status to:</t>
+  </si>
+  <si>
+    <t>TransactionProgress_ClassificationValidation</t>
+  </si>
+  <si>
+    <t>Validating Classification</t>
+  </si>
+  <si>
+    <t>TransactionProgress_ExtractionValidation</t>
+  </si>
+  <si>
+    <t>Validating Data Extraction</t>
+  </si>
+  <si>
+    <t>TestQueue</t>
+  </si>
+  <si>
+    <t>Failed to process document due to:</t>
   </si>
 </sst>
 </file>
@@ -754,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -841,13 +889,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -855,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -863,24 +911,24 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
         <v>79</v>
-      </c>
-      <c r="B7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -904,41 +952,47 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -946,10 +1000,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -957,32 +1011,32 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
         <v>110</v>
-      </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1986,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2043,51 +2097,51 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2129,15 +2183,15 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2150,15 +2204,15 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
@@ -2166,7 +2220,7 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -2174,7 +2228,7 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
@@ -2182,18 +2236,18 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2206,18 +2260,18 @@
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
         <v>65</v>
-      </c>
-      <c r="B24" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2225,28 +2279,28 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -2254,18 +2308,18 @@
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2281,7 +2335,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2295,61 +2349,110 @@
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+    </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>36</v>
       </c>
-      <c r="B40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3293,6 +3396,15 @@
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3324,7 +3436,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3355,13 +3467,13 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
- Added LockFile/UnlockFile log messages - Created a lock/unlock mechanism with GUID instead of datetime
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\GitProjects\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C194B7CB-351D-40C5-82C6-12CDA5032463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C234D-8502-46BE-8749-6F7ACC9F244F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="1920" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -379,6 +379,24 @@
   </si>
   <si>
     <t>Data Extraction finished</t>
+  </si>
+  <si>
+    <t>LogMessage_LockFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locking keyword file: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unlocking keyword file: </t>
+  </si>
+  <si>
+    <t>Unlock complete!</t>
+  </si>
+  <si>
+    <t>LogMessage_UnLockFileFinshed</t>
+  </si>
+  <si>
+    <t>LogMessage_UnLockFileStarted</t>
   </si>
 </sst>
 </file>
@@ -1992,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,43 +2324,64 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-    </row>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>22</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3307,6 +3346,9 @@
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix for AC Data Validation path output argument Added annotations marking the custom retry attempts (for digitize/classify/extract) overriding the default retry counter
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC05BC3-D47B-4E9D-8846-79D386415556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2633605C-CF94-40C4-A476-5730D44D8FD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>RetryInterval</t>
   </si>
   <si>
-    <t>Duration, in seconds, between execution attempts</t>
-  </si>
-  <si>
     <t>ClassifierLearningFilePath</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>StorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>Duration, in seconds, between re-execution attempts</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -908,13 +908,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>136</v>
-      </c>
-      <c r="C3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -922,7 +922,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -930,24 +930,24 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -956,7 +956,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -964,7 +964,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -975,46 +975,46 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1034,10 +1034,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1045,32 +1045,32 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
         <v>101</v>
       </c>
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1019"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2131,40 +2131,40 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2175,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2214,10 +2214,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
         <v>139</v>
-      </c>
-      <c r="B14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2225,15 +2225,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2246,15 +2246,15 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -2281,7 +2281,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2289,7 +2289,7 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,26 +2302,26 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
         <v>85</v>
-      </c>
-      <c r="B27" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,28 +2329,28 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
@@ -2358,18 +2358,18 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2385,7 +2385,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2398,84 +2398,84 @@
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
         <v>111</v>
-      </c>
-      <c r="B37" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" t="s">
         <v>120</v>
-      </c>
-      <c r="B41" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
         <v>116</v>
-      </c>
-      <c r="B42" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" t="s">
         <v>118</v>
-      </c>
-      <c r="B43" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" t="s">
         <v>122</v>
-      </c>
-      <c r="B44" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" t="s">
         <v>126</v>
-      </c>
-      <c r="B45" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
         <v>60</v>
-      </c>
-      <c r="B48" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2500,7 +2500,7 @@
         <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Re-created the lost Config settings; fixed a typo in the Classification endpoint key Re-added the DownloadDirectory Path in Wait For Document Data Validation Action And Resume Merged the Download and Split folders into a single folder Added Config parameter to enable/disable PDF splitting; Default is ON RetryInterval updated to 30s (publish value) Added timeout for LockFile/UnlockFile & made a bit of logic cleanup Removed all custom log fields for now
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2633605C-CF94-40C4-A476-5730D44D8FD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DA3C17-67B7-4F59-BC68-BDAAEDDFFF50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -204,9 +204,6 @@
     <t>WarnMessage_DocumentProcessingFailure</t>
   </si>
   <si>
-    <t>Failed to process document. Exception:</t>
-  </si>
-  <si>
     <t>https://du.uipath.com/ie/invoices</t>
   </si>
   <si>
@@ -411,30 +408,12 @@
     <t>ClassificationEndpoint</t>
   </si>
   <si>
-    <t>Orchestrator folder path to the ActionCatalog</t>
-  </si>
-  <si>
-    <t>Path wihin the Storage Bucket where actions should store data</t>
-  </si>
-  <si>
-    <t>Action Catalog to be used for Classification/Validation actions</t>
-  </si>
-  <si>
-    <t>Name of the Orchestrator Storage Bucket (required when Action Center is used)</t>
-  </si>
-  <si>
     <t>The name of the Orchestrator Queue</t>
   </si>
   <si>
-    <t>Orchestrator folder path to the Queue</t>
-  </si>
-  <si>
     <t>Data\TempFolder</t>
   </si>
   <si>
-    <t>Local folder where the processing job will temporarily store files (split files or downloaded files when using actions)</t>
-  </si>
-  <si>
     <t>TemporaryLocalFolder</t>
   </si>
   <si>
@@ -451,6 +430,42 @@
   </si>
   <si>
     <t>Duration, in seconds, between re-execution attempts</t>
+  </si>
+  <si>
+    <t>Failed to process page range {0} in file {1}. Exception: {2}</t>
+  </si>
+  <si>
+    <t>Action Catalog Name</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used)</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files</t>
+  </si>
+  <si>
+    <t>AutomaticallySplitPDFs</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Parameter dictating whether PDFs containing multiple documents should automatically be split into multiple files or not (setting is case-insensitive)</t>
+  </si>
+  <si>
+    <t>Folder where the job will store its files (split files or downloaded files when using actions)</t>
+  </si>
+  <si>
+    <t>MaxLockTimeout</t>
+  </si>
+  <si>
+    <t>Duration, in seconds, for how long will a job try to lock a training file before giving up and abandoning the training.</t>
   </si>
 </sst>
 </file>
@@ -509,12 +524,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -908,13 +924,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -922,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -930,155 +946,165 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>129</v>
-      </c>
-    </row>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>132</v>
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>140</v>
-      </c>
-      <c r="C12" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
+        <v>90</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-    </row>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="B21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2062,11 +2088,13 @@
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2074,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1019"/>
+  <dimension ref="A1:Z1021"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2131,40 +2159,40 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2172,52 +2200,55 @@
         <v>53</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="3">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2225,15 +2256,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2246,15 +2277,15 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -2281,7 +2312,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2289,7 +2320,7 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,10 +2333,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
         <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2318,10 +2349,10 @@
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,28 +2360,28 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
@@ -2358,18 +2389,18 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2385,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2398,113 +2429,120 @@
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
         <v>110</v>
-      </c>
-      <c r="B37" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s">
-        <v>17</v>
-      </c>
-    </row>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>34</v>
       </c>
-      <c r="B52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3470,6 +3508,8 @@
     <row r="1017" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1018" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Renamed both Main files to remove spaces Cleanup for Config.xlsx Corrections in annotations
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F0D5C6-7835-44EE-90AD-3CC76C3F58A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DDE4D7-7E26-4470-BC2F-4BB1E04122E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>StorageBucketName</t>
   </si>
   <si>
-    <t>TestBucket</t>
-  </si>
-  <si>
     <t>Retrieve your DocumentUnderstanding ApiKey and configure it in an Asset</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
   </si>
   <si>
     <t>Get Transaction Item started</t>
-  </si>
-  <si>
-    <t>TestQueue</t>
   </si>
   <si>
     <t>StorageBucketDirectoryPath</t>
@@ -861,7 +855,7 @@
   <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -936,13 +930,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -950,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -958,36 +952,36 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
         <v>142</v>
-      </c>
-      <c r="B8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -996,7 +990,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1004,69 +998,63 @@
         <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1074,10 +1062,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1085,32 +1073,32 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2171,62 +2159,62 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2268,15 +2256,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2289,15 +2277,15 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -2305,7 +2293,7 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -2313,7 +2301,7 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -2321,18 +2309,18 @@
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2345,26 +2333,26 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
         <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2372,28 +2360,28 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
@@ -2401,18 +2389,18 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2428,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2442,110 +2430,110 @@
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
         <v>131</v>
-      </c>
-      <c r="B45" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
         <v>120</v>
-      </c>
-      <c r="B47" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
         <v>124</v>
-      </c>
-      <c r="B48" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" t="s">
         <v>114</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
         <v>116</v>
-      </c>
-      <c r="B52" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2570,7 +2558,7 @@
         <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3552,7 +3540,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3571,7 +3559,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3602,13 +3590,13 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Renamed both Main files to remove spaces (#16)
Cleanup for Config.xlsx
Corrections in annotations
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/VB/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\VB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F0D5C6-7835-44EE-90AD-3CC76C3F58A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DDE4D7-7E26-4470-BC2F-4BB1E04122E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>StorageBucketName</t>
   </si>
   <si>
-    <t>TestBucket</t>
-  </si>
-  <si>
     <t>Retrieve your DocumentUnderstanding ApiKey and configure it in an Asset</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
   </si>
   <si>
     <t>Get Transaction Item started</t>
-  </si>
-  <si>
-    <t>TestQueue</t>
   </si>
   <si>
     <t>StorageBucketDirectoryPath</t>
@@ -861,7 +855,7 @@
   <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -936,13 +930,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -950,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -958,36 +952,36 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
         <v>142</v>
-      </c>
-      <c r="B8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -996,7 +990,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1004,69 +998,63 @@
         <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1074,10 +1062,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1085,32 +1073,32 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2171,62 +2159,62 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2268,15 +2256,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2289,15 +2277,15 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -2305,7 +2293,7 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -2313,7 +2301,7 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -2321,18 +2309,18 @@
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2345,26 +2333,26 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
         <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2372,28 +2360,28 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
@@ -2401,18 +2389,18 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2428,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2442,110 +2430,110 @@
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
         <v>131</v>
-      </c>
-      <c r="B45" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
         <v>120</v>
-      </c>
-      <c r="B47" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
         <v>124</v>
-      </c>
-      <c r="B48" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" t="s">
         <v>114</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
         <v>116</v>
-      </c>
-      <c r="B52" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2570,7 +2558,7 @@
         <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3552,7 +3540,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3571,7 +3559,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3602,13 +3590,13 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>